<commit_message>
fixed spelling in summary table
</commit_message>
<xml_diff>
--- a/results/Model Scores.xlsx
+++ b/results/Model Scores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utgoy\Desktop\Cornell Tech\Fall 2024\4. ORIE 5750 Applied Machine Learning\Midterm Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utgoy\Desktop\Cornell Tech\Fall 2024\4. ORIE 5750 Applied Machine Learning\Midterm Project\AML_midterm\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF08B7E-AB76-4623-A9EE-5B05238CC73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5628A2E8-0D92-47DA-8ADC-E2CF07B077ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B0D1E02-B35B-418A-BD07-EFBCFFC9A7B3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="19">
   <si>
     <t>Vectorization</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>all-MiniLM-L6-v2</t>
+  </si>
+  <si>
+    <t>Dimensionality Reduction</t>
   </si>
 </sst>
 </file>
@@ -227,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -241,55 +244,64 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,7 +639,7 @@
   <dimension ref="B2:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
@@ -663,29 +675,29 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="12">
         <v>0.85770000000000002</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="12">
         <v>0.85770000000000002</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="15"/>
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
@@ -697,40 +709,40 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="13" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <v>0.84660000000000002</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="8">
         <v>0.84670000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="13" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>0.81610000000000005</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>0.81720000000000004</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="6">
@@ -741,71 +753,71 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="13" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="12">
         <v>0.83040000000000003</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="12">
         <v>0.82899999999999996</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="13" t="s">
+      <c r="B9" s="27"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>0.83950000000000002</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <v>0.83899999999999997</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="13" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <v>0.82150000000000001</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="8">
         <v>0.82130000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <v>0.70709999999999995</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="8">
         <v>0.70850000000000002</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="15"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="12"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
@@ -817,55 +829,55 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="15"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8">
         <v>0.74580000000000002</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="8">
         <v>0.74509999999999998</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="15"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="20" t="s">
+      <c r="B14" s="18"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="12">
         <v>0.75209999999999999</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="12">
         <v>0.75180000000000002</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="15"/>
-      <c r="C15" s="24" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="8">
         <v>0.73670000000000002</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="8">
         <v>0.7379</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="15"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
@@ -877,30 +889,30 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="15"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="13" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8">
         <v>0.79149999999999998</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="8">
         <v>0.79100000000000004</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="16"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="20" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="12">
         <v>0.80079999999999996</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="12">
         <v>0.80059999999999998</v>
       </c>
     </row>
@@ -970,13 +982,13 @@
       </c>
     </row>
     <row r="3" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -988,77 +1000,77 @@
       <c r="G3" s="6">
         <v>0.68610000000000004</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="8">
         <v>0.66</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="8">
         <v>0.64</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="20" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="12">
         <v>0.66739999999999999</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="12">
         <v>0.67059999999999997</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="8">
         <v>0.66</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="8">
         <v>0.64</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="12"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <v>0.64339999999999997</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="8">
         <v>0.64570000000000005</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="8">
         <v>0.62</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="8">
         <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="12"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>0.59130000000000005</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>0.59260000000000002</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="8">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="8">
         <v>0.54</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="12"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1070,79 +1082,79 @@
       <c r="G7" s="6">
         <v>0.7429</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="8">
         <v>0.73</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="8">
         <v>0.73</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="12"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="20" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="12">
         <v>0.74719999999999998</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="12">
         <v>0.74180000000000001</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="8">
         <v>0.72</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="8">
         <v>0.71</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="12"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="13" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>0.73429999999999995</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <v>0.72860000000000003</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="8">
         <v>0.7</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="8">
         <v>0.7</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="12"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="13" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <v>0.68830000000000002</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="8">
         <v>0.68159999999999998</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="8">
         <v>0.69</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="8">
         <v>0.69</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="17" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1154,77 +1166,77 @@
       <c r="G11" s="6">
         <v>0.66420000000000001</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="8">
         <v>0.69</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="8">
         <v>0.67</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="20" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="12">
         <v>0.67920000000000003</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="12">
         <v>0.66439999999999999</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="8">
         <v>0.69</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="8">
         <v>0.67</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8">
         <v>0.65939999999999999</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="8">
         <v>0.64229999999999998</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="8">
         <v>0.67</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="8">
         <v>0.65</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="8">
         <v>0.63529999999999998</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="8">
         <v>0.61670000000000003</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="8">
         <v>0.65</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="8">
         <v>0.63</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="7" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1236,103 +1248,103 @@
       <c r="G15" s="6">
         <v>0.66859999999999997</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="8">
         <v>0.7</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="8">
         <v>0.68</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="20" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="12">
         <v>0.68620000000000003</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="12">
         <v>0.66959999999999997</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="8">
         <v>0.7</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="8">
         <v>0.68</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="13" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8">
         <v>0.66659999999999997</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="8">
         <v>0.64900000000000002</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="8">
         <v>0.68</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="8">
         <v>0.66</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="13" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="8">
         <v>0.64219999999999999</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="8">
         <v>0.62160000000000004</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="8">
         <v>0.66</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="8">
         <v>0.64</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="10">
         <v>0.6</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="10">
         <v>0.55110000000000003</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="10">
         <v>0.54210000000000003</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="10">
         <v>0.45</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1342,79 +1354,79 @@
       <c r="G20" s="6">
         <v>0.67059999999999997</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="8">
         <v>0.6472</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="8">
         <v>0.62039999999999995</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="18"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13" t="s">
+      <c r="B21" s="22"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="8">
         <v>0.66069999999999995</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="8">
         <v>0.62729999999999997</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I21" s="8">
         <v>0.64659999999999995</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="8">
         <v>0.61660000000000004</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="20" t="s">
+      <c r="B22" s="22"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="12">
         <v>0.67259999999999998</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="12">
         <v>0.64510000000000001</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="8">
         <v>0.66059999999999997</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="8">
         <v>0.6341</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="18"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="7" t="s">
+      <c r="B23" s="22"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="8">
         <v>0.61399999999999999</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="8">
         <v>0.56410000000000005</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23" s="8">
         <v>0.70189999999999997</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J23" s="8">
         <v>0.68579999999999997</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="18"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="7"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="2" t="s">
         <v>7</v>
       </c>
@@ -1424,81 +1436,81 @@
       <c r="G24" s="6">
         <v>0.69259999999999999</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="8">
         <v>0.63829999999999998</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="8">
         <v>0.59289999999999998</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="18"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="20" t="s">
+      <c r="B25" s="22"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="12">
         <v>0.6845</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="12">
         <v>0.64959999999999996</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I25" s="8">
         <v>0.70579999999999998</v>
       </c>
-      <c r="J25" s="11">
+      <c r="J25" s="8">
         <v>0.68689999999999996</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="18"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="13" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="8">
         <v>0.69589999999999996</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="8">
         <v>0.66410000000000002</v>
       </c>
-      <c r="I26" s="11">
+      <c r="I26" s="8">
         <v>0.7167</v>
       </c>
-      <c r="J26" s="11">
+      <c r="J26" s="8">
         <v>0.70089999999999997</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="18"/>
-      <c r="C27" s="7" t="s">
+      <c r="B27" s="22"/>
+      <c r="C27" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="8">
         <v>0.69650000000000001</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="8">
         <v>0.70079999999999998</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I27" s="8">
         <v>0.62870000000000004</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="8">
         <v>0.58540000000000003</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="18"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
       <c r="E28" s="2" t="s">
         <v>7</v>
       </c>
@@ -1508,79 +1520,79 @@
       <c r="G28" s="6">
         <v>0.78790000000000004</v>
       </c>
-      <c r="I28" s="11">
+      <c r="I28" s="8">
         <v>0.70409999999999995</v>
       </c>
-      <c r="J28" s="11">
+      <c r="J28" s="8">
         <v>0.67269999999999996</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="18"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="13" t="s">
+      <c r="B29" s="22"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="8">
         <v>0.76259999999999994</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="8">
         <v>0.76549999999999996</v>
       </c>
-      <c r="I29" s="11">
+      <c r="I29" s="8">
         <v>0.70250000000000001</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="8">
         <v>0.66849999999999998</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="18"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="20" t="s">
+      <c r="B30" s="22"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="12">
         <v>0.76870000000000005</v>
       </c>
-      <c r="G30" s="21">
+      <c r="G30" s="12">
         <v>0.77190000000000003</v>
       </c>
-      <c r="I30" s="11">
+      <c r="I30" s="8">
         <v>0.71679999999999999</v>
       </c>
-      <c r="J30" s="11">
+      <c r="J30" s="8">
         <v>0.68710000000000004</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="18"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="12" t="s">
+      <c r="B31" s="22"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="8">
         <v>0.64770000000000005</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="8">
         <v>0.59409999999999996</v>
       </c>
-      <c r="I31" s="11">
+      <c r="I31" s="8">
         <v>0.62880000000000003</v>
       </c>
-      <c r="J31" s="11">
+      <c r="J31" s="8">
         <v>0.58520000000000005</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="18"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="12"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="17"/>
       <c r="E32" s="2" t="s">
         <v>7</v>
       </c>
@@ -1590,50 +1602,50 @@
       <c r="G32" s="6">
         <v>0.70609999999999995</v>
       </c>
-      <c r="I32" s="11">
+      <c r="I32" s="8">
         <v>0.70309999999999995</v>
       </c>
-      <c r="J32" s="11">
+      <c r="J32" s="8">
         <v>0.6714</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="18"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="13" t="s">
+      <c r="B33" s="22"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="8">
         <v>0.7097</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="8">
         <v>0.67279999999999995</v>
       </c>
-      <c r="I33" s="11">
+      <c r="I33" s="8">
         <v>0.7016</v>
       </c>
-      <c r="J33" s="11">
+      <c r="J33" s="8">
         <v>0.66769999999999996</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="19"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="20" t="s">
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="12">
         <v>0.72240000000000004</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="12">
         <v>0.69020000000000004</v>
       </c>
-      <c r="I34" s="11">
+      <c r="I34" s="8">
         <v>0.71609999999999996</v>
       </c>
-      <c r="J34" s="11">
+      <c r="J34" s="8">
         <v>0.68679999999999997</v>
       </c>
     </row>

</xml_diff>